<commit_message>
Added Self-Hosted Password Manager V2
</commit_message>
<xml_diff>
--- a/Self-Hosted Password Manager/Self-Hosted Password Manager with Linode.xlsx
+++ b/Self-Hosted Password Manager/Self-Hosted Password Manager with Linode.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github Projects\Linode Server\Linode-Project\Self-Hosted Password Manager\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2. Github Projects\Linode Server\Linode-Projects\Self-Hosted Password Manager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0E7FD31-C717-4171-A577-5D75955D4F75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C4285D6-4040-4AF9-A555-FDB242BC73F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9CD1A0AF-48DE-48CF-A889-32A4450B4B5E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="3" xr2:uid="{9CD1A0AF-48DE-48CF-A889-32A4450B4B5E}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="3" r:id="rId1"/>
     <sheet name="Setting up Linode Server" sheetId="1" r:id="rId2"/>
-    <sheet name="Setting up Passbolt with Docker" sheetId="2" r:id="rId3"/>
+    <sheet name="Setting up Passbolt Docker V1" sheetId="2" r:id="rId3"/>
+    <sheet name="Setting up Passbolt Docker V2" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,8 +38,170 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata">
+  <metadataTypes count="1">
+    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLRICHVALUE" count="15">
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="0"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="2"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="3"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="4"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="5"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="6"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="7"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="8"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="9"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="10"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="11"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="12"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="13"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="14"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <valueMetadata count="15">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+    <bk>
+      <rc t="1" v="1"/>
+    </bk>
+    <bk>
+      <rc t="1" v="2"/>
+    </bk>
+    <bk>
+      <rc t="1" v="3"/>
+    </bk>
+    <bk>
+      <rc t="1" v="4"/>
+    </bk>
+    <bk>
+      <rc t="1" v="5"/>
+    </bk>
+    <bk>
+      <rc t="1" v="6"/>
+    </bk>
+    <bk>
+      <rc t="1" v="7"/>
+    </bk>
+    <bk>
+      <rc t="1" v="8"/>
+    </bk>
+    <bk>
+      <rc t="1" v="9"/>
+    </bk>
+    <bk>
+      <rc t="1" v="10"/>
+    </bk>
+    <bk>
+      <rc t="1" v="11"/>
+    </bk>
+    <bk>
+      <rc t="1" v="12"/>
+    </bk>
+    <bk>
+      <rc t="1" v="13"/>
+    </bk>
+    <bk>
+      <rc t="1" v="14"/>
+    </bk>
+  </valueMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="86">
   <si>
     <t>In this Tap, shows on how to set up Password Manager with Passbolt</t>
   </si>
@@ -353,6 +516,144 @@
   </si>
   <si>
     <t>Overall: $7.00/Month</t>
+  </si>
+  <si>
+    <t>Year 2024 (Version 1)</t>
+  </si>
+  <si>
+    <t>Year 2025 (Version 2)</t>
+  </si>
+  <si>
+    <t>Step 1: Install necessary Packages "sudo apt install -y \
+  ca-certificates \
+  curl \
+  gnupg \
+  lsb-release
+ca-certificates: Installs trusted root SSL/TLS certificates.
+curl: A command-line tool to download or send data via URLs.
+gnupg: Provides GPG (GNU Privacy Guard) tools. Verify cryptographic signatures, Import repository signing keys abd Critical for secure package installation (checking authenticity).
+lsb-release: Lets your system report distribution information.</t>
+  </si>
+  <si>
+    <t>Step 2: Proceed with "sudo mkdir -p /etc/apt/keyrings"
+-p: Means “parents”. It creates any missing parent directories automatically and does not throw an error if the directory already exists.
+/etc/apt/keyrings: This is the standard location for storing APT repository signing keys.</t>
+  </si>
+  <si>
+    <t>Step 3: Once done, type in "curl -fsSL https://download.docker.com/linux/ubuntu/gpg | \
+  sudo gpg --dearmor -o /etc/apt/keyrings/docker.gpg"
+This command securely installs Docker’s signing key so your system can verify that Docker packages are authentic and untampered.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Step 4: Once done, type in "echo "deb [arch=$(dpkg --print-architecture) signed-by=/etc/apt/keyrings/docker.gpg] \
+https://download.docker.com/linux/ubuntu \
+$(lsb_release -cs) stable" | \
+  sudo tee /etc/apt/sources.list.d/docker.list &gt; /dev/null"
+echo "deb ... stable": Prints a repository definition line.
+deb: binary packages repository
+arch=$(dpkg --print-architecture): Dynamically inserts your CPU architecture.
+signed-by=/etc/apt/keyrings/docker.gpg: To only trust packages from the repo if thet are signed with the key
+https://download.docker.com/linux/ubuntu: Docker's official Ubuntu repository URL
+$(lsb_release -cs): Insert Ubuntu codename
+stable: Selecr Docker's stable release channel
+echo "..." | sudo tee /etc/apt/sources.list.d/docker.list: Write the file with correct permissions
+&gt; /dev/null: Keeps terminal clean &amp; suppresses tee output
+</t>
+  </si>
+  <si>
+    <t>Step 6: Make a directory "mkdir passbolt" and cd into the directory</t>
+  </si>
+  <si>
+    <t>Step 5: Do a "sudo apt update" and install the docker packages "sudo apt install -y \
+  docker-ce \
+  docker-ce-cli \
+  containerd.io \
+  docker-compose-plugin"
+docker-ce: Docker Community Edition, which resposible for running containers and managing images, networks and volumes.
+docker-ce-cli: Docker Command Line Interface, which provides the docker command.
+containerd.io: Run containers and handles image pulling, container lifecycle and resource isolation.
+docker-compose-plugin: Replace old docker from Version 1.</t>
+  </si>
+  <si>
+    <t>Step 5.1: To start docker immediately and configure the ddocker to start automatically on every system boot, use "sudo systemctl enable --now docker"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Step 7: type in "wget https://download.passbolt.com/ce/docker/docker-compose-ce.yaml" </t>
+  </si>
+  <si>
+    <t>Step 2: Add traefik service to handle https by using:
+version: '3.7'
+services:
+  db:
+    ...
+  passbolt:
+    ...
+----&gt;
+  traefik:
+    image: traefik:v2.11
+    restart: always
+    ports:
+      - 80:80
+      - 443:443
+    volumes:
+      - /var/run/docker.sock:/var/run/docker.sock:ro
+      - ./traefik.yaml:/traefik.yaml:ro
+      - ./conf/:/etc/traefik/conf
+      - ./shared/:/shared
+Do note to remove the duplicate ports 80:80 and 443:443 within the file.</t>
+  </si>
+  <si>
+    <t>Step 8: Open and edit the docker-compose-ce.yaml file with "nano docker-compose-ce.yaml"</t>
+  </si>
+  <si>
+    <t>Step 9: In the Yaml file, locate Environment &gt; APP_FULL_BASE_URL and then change the URL to https://&lt;reverse DNS of Linode&gt;</t>
+  </si>
+  <si>
+    <t>Step 10: Then save the file</t>
+  </si>
+  <si>
+    <t>Step 11: Run "docker compose -f docker-compose-ce.yaml up -d"</t>
+  </si>
+  <si>
+    <t>Step 12: Type "Docker ps" to check the running dockers</t>
+  </si>
+  <si>
+    <t>Step 8: Once done configuring, type in "docker compose -f docker-compose-ce.yaml up -d"</t>
+  </si>
+  <si>
+    <t>Step 1: Once done with configuration, we now need to create admin user by using:
+docker compose -f docker-compose-ce.yaml exec passbolt su -m -c "/usr/share/php/passbolt/bin/cake \
+                                passbolt register_user \
+                                -u &lt;your@email.com&gt; \
+                                -f &lt;yourname&gt; \
+                                -l &lt;surname&gt; \
+                                -r admin" -s /bin/sh www-data
+Do change, your email address, yourname &amp; surname. then press enter.</t>
+  </si>
+  <si>
+    <t>Configuring JWT/RSA for Passbolt Mobile</t>
+  </si>
+  <si>
+    <t>Step 1: Generate JWT keys by using "docker exec -it passbolt-passbolt-1 sh -lc "bin/cake passbolt create_jwt_keys""
+docker exec: runs a command inside a running container (Do not restart or recreate the container)
+-it: -i interactive and -t allocates a pseudo-terminal which allows sheel comamnds to run properly
+passbolt-passbolt-1: The container name
+sh -lc "…": Start a shell inside the container which -l login shell and -c which run the command inside the quotes
+"bin/cake passbolt create_jwt_keys": bin/cake is a cakePHP's command-line tool and Passbolt is built on CakePHP. create_jwt_keys, is that it generates the JWT private key (jwt.key) and JWT public key (jwt.pem)</t>
+  </si>
+  <si>
+    <t>Step 2: To verify if the key exist by running "docker exec -it passbolt-passbolt-1 sh -lc "ls -lah /etc/passbolt/jwt""</t>
+  </si>
+  <si>
+    <t>Step 3: Once generated the key, change the ownership to www-data so that Passbolt can actually use the JWT keys by typing "docker exec -it passbolt-passbolt-1 sh -lc "chown -R www-data:www-data /etc/passbolt/jwt""
+chown -R www-data:www-data /etc/passbolt/jwt: Where chown is to change file owner, -R make it recursive and applies to /etc/passbolt/jwt all files inside it. www-data:www-data is the owner : group which the Apache / PHP-FPM runs as in which the passbolt is using.</t>
+  </si>
+  <si>
+    <t>Step 4: Verify the change of ownership by running the same command "docker exec -it passbolt-passbolt-1 sh -lc "ls -lah /etc/passbolt/jwt""</t>
+  </si>
+  <si>
+    <t>Step 5: Once done, we need to restart passbolt by using the command "docker compose -f docker-compose-ce.yaml restart passbolt"
+Then you are done, and ensure to test it out!</t>
   </si>
 </sst>
 </file>
@@ -616,7 +917,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -662,24 +963,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -716,6 +999,24 @@
     <xf numFmtId="8" fontId="5" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -736,6 +1037,19 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1496,13 +1810,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1569,13 +1883,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1642,13 +1956,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1715,13 +2029,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1788,13 +2102,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1861,13 +2175,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1934,13 +2248,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2007,13 +2321,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2080,13 +2394,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2153,13 +2467,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2226,13 +2540,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2299,13 +2613,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2372,13 +2686,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2442,6 +2756,944 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Rectangle 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{384CA155-49FB-4C1B-B0C2-3742C72C97E5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4221480" y="2766060"/>
+          <a:ext cx="3939540" cy="365760"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:blipFill dpi="0" rotWithShape="1">
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </a:blipFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-SG" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Rectangle 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4999F80A-F8B5-4E4B-9C3D-3DABD0274A27}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4221480" y="3314700"/>
+          <a:ext cx="3939540" cy="1211580"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:blipFill dpi="0" rotWithShape="1">
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </a:blipFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-SG" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Rectangle 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7F9A8DA7-60D3-4F49-B498-BFCE3E1CA70B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4221480" y="4526280"/>
+          <a:ext cx="3939540" cy="518160"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:blipFill dpi="0" rotWithShape="1">
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </a:blipFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-SG" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Rectangle 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9DA45453-E9F0-4C54-B0FD-A210687184E0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4221480" y="9494520"/>
+          <a:ext cx="3939540" cy="2956560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:blipFill dpi="0" rotWithShape="1">
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </a:blipFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-SG" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Rectangle 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{487EFC98-D142-4187-A2C2-D371DDD58C77}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4221480" y="12451080"/>
+          <a:ext cx="3939540" cy="2956560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:blipFill dpi="0" rotWithShape="1">
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </a:blipFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-SG" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Rectangle 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF524801-1529-4D3F-965A-30EB0BB0B8F0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4221480" y="15407640"/>
+          <a:ext cx="3939540" cy="4983480"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:blipFill dpi="0" rotWithShape="1">
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </a:blipFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-SG" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="Rectangle 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C5E9E60-B5BA-4732-86F5-2A87A639CD14}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4221480" y="24490680"/>
+          <a:ext cx="3939540" cy="4739640"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:blipFill dpi="0" rotWithShape="1">
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </a:blipFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-SG" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="Rectangle 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D703206B-05EE-47F4-BC2D-F73A1BE1D1A0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4221480" y="29230320"/>
+          <a:ext cx="3939540" cy="3680460"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:blipFill dpi="0" rotWithShape="1">
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </a:blipFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-SG" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="Rectangle 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC0905D3-10F9-44C9-936C-579E0B4183DF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4221480" y="36019740"/>
+          <a:ext cx="3939540" cy="2065020"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:blipFill dpi="0" rotWithShape="1">
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </a:blipFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-SG" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1352549</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>490538</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2628899</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>757238</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="TextBox 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DCCF6B71-17D6-D74C-FB7C-19A836DFF8C0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9710737" y="64165163"/>
+          <a:ext cx="1276350" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-SG" sz="1100"/>
+            <a:t>After</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1162050</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>581026</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2438400</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>847726</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="TextBox 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E98FB3C6-095F-4AD1-A220-2433A3BBE011}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5381625" y="64255651"/>
+          <a:ext cx="1276350" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-SG" sz="1100"/>
+            <a:t>Before</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
+<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
+  <global>
+    <keyFlags>
+      <key name="_Self">
+        <flag name="ExcludeFromFile" value="1"/>
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_DisplayString">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Flags">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Format">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_SubLabel">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Attribution">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Icon">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Display">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_CanonicalPropertyNames">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_ClassificationId">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+    </keyFlags>
+  </global>
+</rvTypesInfo>
+</file>
+
+<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="15">
+  <rv s="0">
+    <v>0</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>1</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>2</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>3</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>4</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>5</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>6</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>7</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>8</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>9</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>10</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>11</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>12</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>13</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>14</v>
+    <v>5</v>
+  </rv>
+</rvData>
+</file>
+
+<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <s t="_localImage">
+    <k n="_rvRel:LocalImageIdentifier" t="i"/>
+    <k n="CalcOrigin" t="i"/>
+  </s>
+</rvStructures>
+</file>
+
+<file path=xl/richData/richValueRel.xml><?xml version="1.0" encoding="utf-8"?>
+<richValueRels xmlns="http://schemas.microsoft.com/office/spreadsheetml/2022/richvaluerel" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rel r:id="rId1"/>
+  <rel r:id="rId2"/>
+  <rel r:id="rId3"/>
+  <rel r:id="rId4"/>
+  <rel r:id="rId5"/>
+  <rel r:id="rId6"/>
+  <rel r:id="rId7"/>
+  <rel r:id="rId8"/>
+  <rel r:id="rId9"/>
+  <rel r:id="rId10"/>
+  <rel r:id="rId11"/>
+  <rel r:id="rId12"/>
+  <rel r:id="rId13"/>
+  <rel r:id="rId14"/>
+  <rel r:id="rId15"/>
+</richValueRels>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2763,7 +4015,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46BBD57B-C54B-4747-8B2A-240F1FB947C8}">
   <dimension ref="B2:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
@@ -2805,74 +4057,74 @@
       <c r="E4" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="H4" s="23" t="s">
+      <c r="H4" s="17" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="5" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="30">
+      <c r="D5" s="24">
         <v>0</v>
       </c>
-      <c r="E5" s="30">
+      <c r="E5" s="24">
         <v>0</v>
       </c>
-      <c r="H5" s="23"/>
+      <c r="H5" s="17"/>
     </row>
     <row r="6" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="25"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
-      <c r="H6" s="23"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="H6" s="17"/>
     </row>
     <row r="7" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="25"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
-      <c r="H7" s="23"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="H7" s="17"/>
     </row>
     <row r="8" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="25"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="31"/>
-      <c r="H8" s="23"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+      <c r="H8" s="17"/>
     </row>
     <row r="9" spans="2:8" ht="54.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="26"/>
-      <c r="C9" s="29"/>
-      <c r="D9" s="32"/>
-      <c r="E9" s="32"/>
-      <c r="H9" s="23"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
+      <c r="H9" s="17"/>
     </row>
     <row r="10" spans="2:8" ht="93.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="27" t="s">
+      <c r="C10" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="33" t="s">
+      <c r="D10" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="E10" s="30" t="s">
+      <c r="E10" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="H10" s="23"/>
+      <c r="H10" s="17"/>
     </row>
     <row r="11" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="26"/>
-      <c r="C11" s="29"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="32"/>
-      <c r="H11" s="23"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="26"/>
+      <c r="H11" s="17"/>
     </row>
     <row r="12" spans="2:8" ht="45.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="10" t="s">
@@ -2887,7 +4139,7 @@
       <c r="E12" s="12">
         <v>0</v>
       </c>
-      <c r="H12" s="23"/>
+      <c r="H12" s="17"/>
     </row>
     <row r="13" spans="2:8" ht="45.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="13"/>
@@ -2896,7 +4148,7 @@
       <c r="E13" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="H13" s="23"/>
+      <c r="H13" s="17"/>
     </row>
     <row r="16" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="17" spans="2:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -2907,19 +4159,19 @@
       <c r="D17" s="16"/>
       <c r="E17" s="16"/>
       <c r="F17" s="16"/>
-      <c r="H17" s="17" t="s">
+      <c r="H17" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="I17" s="17"/>
+      <c r="I17" s="29"/>
     </row>
     <row r="18" spans="2:9" ht="118.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="20" t="s">
+      <c r="B18" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="C18" s="21"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="22"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="34"/>
       <c r="H18" s="15" t="s">
         <v>55</v>
       </c>
@@ -2941,19 +4193,24 @@
       <c r="I21" s="16"/>
     </row>
     <row r="22" spans="2:9" ht="164.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="18" t="s">
+      <c r="B22" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="C22" s="19"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="19"/>
-      <c r="H22" s="19"/>
-      <c r="I22" s="19"/>
+      <c r="C22" s="31"/>
+      <c r="D22" s="31"/>
+      <c r="E22" s="31"/>
+      <c r="F22" s="31"/>
+      <c r="G22" s="31"/>
+      <c r="H22" s="31"/>
+      <c r="I22" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="B21:I21"/>
+    <mergeCell ref="B22:I22"/>
+    <mergeCell ref="B18:F18"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="H4:H13"/>
     <mergeCell ref="B5:B9"/>
@@ -2964,11 +4221,6 @@
     <mergeCell ref="C10:C11"/>
     <mergeCell ref="D10:D11"/>
     <mergeCell ref="E10:E11"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="B21:I21"/>
-    <mergeCell ref="B22:I22"/>
-    <mergeCell ref="B18:F18"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="I18" r:id="rId1" xr:uid="{6B294BFB-031A-4A0E-B3F0-E8C54BC4AF93}"/>
@@ -3103,10 +4355,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AEF3A83-BD0E-4F0C-8BBE-FDB4AA913FCF}">
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3121,177 +4373,509 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="37" t="s">
+      <c r="A2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="37"/>
       <c r="B3" s="37"/>
       <c r="C3" s="37"/>
     </row>
-    <row r="4" spans="1:3" ht="73.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="37"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
+    </row>
+    <row r="5" spans="1:3" ht="73.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+    <row r="7" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="95.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
+    <row r="11" spans="1:3" ht="95.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
+    <row r="12" spans="1:3" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="38" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="39"/>
-      <c r="C12" s="39"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="38"/>
       <c r="B13" s="39"/>
       <c r="C13" s="39"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="38"/>
+      <c r="B14" s="39"/>
+      <c r="C14" s="39"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="307.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
+    <row r="16" spans="1:3" ht="307.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="232.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="40" t="s">
+    <row r="17" spans="1:7" ht="232.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="40" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="232.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="41"/>
-    </row>
-    <row r="18" spans="1:7" ht="392.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="40" t="s">
+    <row r="18" spans="1:7" ht="232.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="41"/>
+    </row>
+    <row r="19" spans="1:7" ht="392.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="40" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="294" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="41"/>
-      <c r="G19" s="40"/>
-    </row>
-    <row r="20" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
+    <row r="20" spans="1:7" ht="294" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="41"/>
+      <c r="G20" s="40"/>
+    </row>
+    <row r="21" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G20" s="41"/>
-    </row>
-    <row r="21" spans="1:7" ht="373.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
+      <c r="G21" s="41"/>
+    </row>
+    <row r="22" spans="1:7" ht="373.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="289.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
+    <row r="23" spans="1:7" ht="289.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A23" s="3" t="s">
+    <row r="24" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="36" t="s">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="B24" s="36"/>
-      <c r="C24" s="36"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="36"/>
       <c r="B25" s="36"/>
       <c r="C25" s="36"/>
     </row>
-    <row r="26" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
-      <c r="A26" s="6" t="s">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="36"/>
+      <c r="B26" s="36"/>
+      <c r="C26" s="36"/>
+    </row>
+    <row r="27" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A27" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="162.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="5" t="s">
+    <row r="28" spans="1:7" ht="162.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="117.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="5" t="s">
+    <row r="29" spans="1:7" ht="117.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33" s="7" t="s">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" s="7" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A34" s="4" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" s="4" t="s">
         <v>24</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A24:C25"/>
-    <mergeCell ref="A2:C3"/>
-    <mergeCell ref="A12:C13"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="A25:C26"/>
+    <mergeCell ref="A3:C4"/>
+    <mergeCell ref="A13:C14"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A19:A20"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A33" r:id="rId1" xr:uid="{5B225E25-040C-4516-8C00-27D4DA7225D6}"/>
-    <hyperlink ref="A34" r:id="rId2" xr:uid="{229A9DDE-E181-464E-8B12-F1E6B0ED6040}"/>
-    <hyperlink ref="A35" r:id="rId3" xr:uid="{0B08AC8E-9D13-46A3-816A-0C3E6234BFBD}"/>
+    <hyperlink ref="A34" r:id="rId1" xr:uid="{5B225E25-040C-4516-8C00-27D4DA7225D6}"/>
+    <hyperlink ref="A35" r:id="rId2" xr:uid="{229A9DDE-E181-464E-8B12-F1E6B0ED6040}"/>
+    <hyperlink ref="A36" r:id="rId3" xr:uid="{0B08AC8E-9D13-46A3-816A-0C3E6234BFBD}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
+  <drawing r:id="rId5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FD3338F-D859-4B68-85FC-B9C246D736F0}">
+  <dimension ref="A1:G48"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="80" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="61.5546875" customWidth="1"/>
+    <col min="2" max="2" width="60.33203125" customWidth="1"/>
+    <col min="3" max="3" width="63.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="37"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
+    </row>
+    <row r="5" spans="1:3" ht="252.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" s="44" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="156" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" s="44" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="133.80000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7" s="44" t="e" vm="3">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="409.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B8" s="44" t="e" vm="4">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="270" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" s="44" t="e" vm="5">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="127.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B10" s="44" t="e" vm="6">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B11" s="45"/>
+    </row>
+    <row r="12" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B12" s="45"/>
+    </row>
+    <row r="13" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B13" s="45"/>
+    </row>
+    <row r="14" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B14" s="45"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B15" s="45"/>
+    </row>
+    <row r="16" spans="1:3" ht="95.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B16" s="45"/>
+    </row>
+    <row r="17" spans="1:7" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="39"/>
+      <c r="C18" s="39"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="38"/>
+      <c r="B19" s="39"/>
+      <c r="C19" s="39"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="358.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B21" s="44" t="e" vm="7">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="232.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="45"/>
+    </row>
+    <row r="23" spans="1:7" ht="232.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="41"/>
+      <c r="B23" s="45"/>
+    </row>
+    <row r="24" spans="1:7" ht="392.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" s="45"/>
+    </row>
+    <row r="25" spans="1:7" ht="294" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="41"/>
+      <c r="B25" s="45"/>
+      <c r="G25" s="40"/>
+    </row>
+    <row r="26" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B26" s="45"/>
+      <c r="G26" s="41"/>
+    </row>
+    <row r="27" spans="1:7" ht="373.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B27" s="45"/>
+    </row>
+    <row r="28" spans="1:7" ht="289.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B28" s="45"/>
+    </row>
+    <row r="29" spans="1:7" ht="142.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B29" s="46" t="e" vm="8">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="B30" s="36"/>
+      <c r="C30" s="36"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="36"/>
+      <c r="B31" s="36"/>
+      <c r="C31" s="36"/>
+    </row>
+    <row r="32" spans="1:7" ht="199.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B32" s="44" t="e" vm="9">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="162.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B33" s="45"/>
+    </row>
+    <row r="34" spans="1:3" ht="143.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B34" s="44" t="e" vm="10">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="37" t="s">
+        <v>80</v>
+      </c>
+      <c r="B35" s="37"/>
+      <c r="C35" s="37"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="37"/>
+      <c r="B36" s="37"/>
+      <c r="C36" s="37"/>
+    </row>
+    <row r="37" spans="1:3" ht="262.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="43" t="s">
+        <v>81</v>
+      </c>
+      <c r="B37" s="46" t="e" vm="11">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A38" s="42" t="s">
+        <v>82</v>
+      </c>
+      <c r="B38" s="45"/>
+    </row>
+    <row r="39" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A39" s="43" t="s">
+        <v>83</v>
+      </c>
+      <c r="B39" s="44" t="e" vm="12">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="132.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="43" t="s">
+        <v>84</v>
+      </c>
+      <c r="B40" s="45" t="e" vm="13">
+        <v>#VALUE!</v>
+      </c>
+      <c r="C40" s="45" t="e" vm="14">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="118.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="43" t="s">
+        <v>85</v>
+      </c>
+      <c r="B41" s="44" t="e" vm="15">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A35:C36"/>
+    <mergeCell ref="A3:C4"/>
+    <mergeCell ref="A18:C19"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="G25:G26"/>
+    <mergeCell ref="A30:C31"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A46" r:id="rId1" xr:uid="{C766D03E-A956-419D-9325-E83CD261FCF7}"/>
+    <hyperlink ref="A47" r:id="rId2" xr:uid="{D9EF6B8A-5635-475A-9B4D-63DC1BB46FF8}"/>
+    <hyperlink ref="A48" r:id="rId3" xr:uid="{7773235E-0FE6-4D7A-9B8F-574E9020B49B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>

</xml_diff>